<commit_message>
Corrected printing issue, some naming mistakes
</commit_message>
<xml_diff>
--- a/Tables_Figures/output/table17_SR_uninflected_anovas.xlsx
+++ b/Tables_Figures/output/table17_SR_uninflected_anovas.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Effect</t>
   </si>
@@ -24,27 +24,6 @@
   </si>
   <si>
     <t>F2</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
   </si>
   <si>
     <t>Local Noun Number</t>
@@ -159,20 +138,19 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1"/>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -180,140 +158,119 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="n">
+        <v>6.532</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="n">
-        <v>6.532</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D2" t="n">
+        <v>5.123</v>
+      </c>
+      <c r="E2" t="s">
         <v>18</v>
-      </c>
-      <c r="E2" t="n">
-        <v>5.123</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="n">
+        <v>2.1913</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="n">
-        <v>2.1913</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D3" t="n">
+        <v>0.4529</v>
+      </c>
+      <c r="E3" t="s">
         <v>19</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.4529</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="n">
+        <v>0.028716</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="n">
-        <v>0.028716</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="D4" t="n">
+        <v>0.03394</v>
+      </c>
+      <c r="E4" t="s">
         <v>20</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.03394</v>
-      </c>
-      <c r="F4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="n">
+        <v>38.38</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="n">
-        <v>38.38</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="D5" t="n">
+        <v>11.596</v>
+      </c>
+      <c r="E5" t="s">
         <v>21</v>
-      </c>
-      <c r="E5" t="n">
-        <v>11.596</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="n">
+        <v>1.0063</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="n">
-        <v>1.0063</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="D6" t="n">
+        <v>1.4148</v>
+      </c>
+      <c r="E6" t="s">
         <v>22</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1.4148</v>
-      </c>
-      <c r="F6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="n">
+        <v>9.778</v>
+      </c>
+      <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="n">
-        <v>9.778</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="D7" t="n">
+        <v>4.535</v>
+      </c>
+      <c r="E7" t="s">
         <v>23</v>
-      </c>
-      <c r="E7" t="n">
-        <v>4.535</v>
-      </c>
-      <c r="F7" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="n">
+        <v>0.05735</v>
+      </c>
+      <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="n">
-        <v>0.05735</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="D8" t="n">
+        <v>0.04846</v>
+      </c>
+      <c r="E8" t="s">
         <v>24</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.04846</v>
-      </c>
-      <c r="F8" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>